<commit_message>
add empty rows report dev
</commit_message>
<xml_diff>
--- a/public/Format_Dev.xlsx
+++ b/public/Format_Dev.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E37D62-1E45-4FF5-9CE0-3890E5CBB390}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16C41B2-C500-49C9-81C0-870C31C704EC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -899,14 +899,14 @@
   <dimension ref="B1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="15.88671875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="40.5546875" style="6" customWidth="1"/>
     <col min="4" max="4" width="16.88671875" style="6" customWidth="1"/>
     <col min="5" max="5" width="14" style="6" customWidth="1"/>
     <col min="6" max="6" width="14.109375" style="6" customWidth="1"/>

</xml_diff>